<commit_message>
Signals and Registers Mapping ready for Baseline Milestone
</commit_message>
<xml_diff>
--- a/Mapping/Register and Signal Mapping.xlsx
+++ b/Mapping/Register and Signal Mapping.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1531" uniqueCount="435">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1675" uniqueCount="499">
   <si>
     <t>Signal</t>
   </si>
@@ -1325,6 +1325,198 @@
   </si>
   <si>
     <t>3000_0281</t>
+  </si>
+  <si>
+    <t>Pri_Input_Payload_Check</t>
+  </si>
+  <si>
+    <t>Ter_Input_Payload_Check</t>
+  </si>
+  <si>
+    <t>Sec_Input_Payload_Check</t>
+  </si>
+  <si>
+    <t>Pri_Output_Payload_Check</t>
+  </si>
+  <si>
+    <t>Sec_Output_Payload_Check</t>
+  </si>
+  <si>
+    <t>Ter_Output_Payload_Check</t>
+  </si>
+  <si>
+    <t>Temp_Max_001</t>
+  </si>
+  <si>
+    <t>Temp_Min_001</t>
+  </si>
+  <si>
+    <t>Temp_Max_002</t>
+  </si>
+  <si>
+    <t>Temp_Min_002</t>
+  </si>
+  <si>
+    <t>Temp_Max_003</t>
+  </si>
+  <si>
+    <t>Temp_Min_003</t>
+  </si>
+  <si>
+    <t>Ex_Sys_Course_Cor_Ts_D</t>
+  </si>
+  <si>
+    <t>Ex_Sys_Course_Cor_Ts_E</t>
+  </si>
+  <si>
+    <t>Ex_Sys_Com_Check_Ts_D</t>
+  </si>
+  <si>
+    <t>Ex_Sys_Com_Check_Ts_E</t>
+  </si>
+  <si>
+    <t>Sim_Run_Ts_In</t>
+  </si>
+  <si>
+    <t>Sim_Run_Ts_L</t>
+  </si>
+  <si>
+    <t>Rtec_Switch_Mon</t>
+  </si>
+  <si>
+    <t>Ap_Reset_Switch_Ts_D</t>
+  </si>
+  <si>
+    <t>Pri_Pressure_Enabler_Run</t>
+  </si>
+  <si>
+    <t>Sec_Pressure_Enabler_Run</t>
+  </si>
+  <si>
+    <t>Ter_Pressure_Enabler_Run</t>
+  </si>
+  <si>
+    <t>Local_Area_Range_Check_Ts_E_2</t>
+  </si>
+  <si>
+    <t>Local_Area_Range_Check_Ts_E_1</t>
+  </si>
+  <si>
+    <t>Local_Area_Range_Check_Ts_E_3</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_1</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_2</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_3</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_4</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_5</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_6</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_7</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_8</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_9</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_10</t>
+  </si>
+  <si>
+    <t>Check_Ts_In_11</t>
+  </si>
+  <si>
+    <t>Value_Check_Nvram_1</t>
+  </si>
+  <si>
+    <t>Value_Check_Nvram_2</t>
+  </si>
+  <si>
+    <t>Value_Check_Sram_1</t>
+  </si>
+  <si>
+    <t>Value_Check_Sram_2</t>
+  </si>
+  <si>
+    <t>Value_Check_Flash_1</t>
+  </si>
+  <si>
+    <t>Value_Check_Flash_2</t>
+  </si>
+  <si>
+    <t>LP_Raw_Distance</t>
+  </si>
+  <si>
+    <t>LP_Raw_Distance_Max</t>
+  </si>
+  <si>
+    <t>LP_Raw_Distance_Min</t>
+  </si>
+  <si>
+    <t>LP_Raw_Time</t>
+  </si>
+  <si>
+    <t>LP_Raw_Distance_Time</t>
+  </si>
+  <si>
+    <t>LP_Raw_Distance_Time_Max</t>
+  </si>
+  <si>
+    <t>LP_Raw_Distance_Time_Min</t>
+  </si>
+  <si>
+    <t>Raw_Acceleration_Nx_Value</t>
+  </si>
+  <si>
+    <t>Raw_Acceleration_Nx_Max</t>
+  </si>
+  <si>
+    <t>Projectile_Angle_Raw</t>
+  </si>
+  <si>
+    <t>Projectile_Angle_Max</t>
+  </si>
+  <si>
+    <t>Projectile_Correction_Signal</t>
+  </si>
+  <si>
+    <t>Err_Signal_Radar_Comms</t>
+  </si>
+  <si>
+    <t>Drop_Time_End_Reg</t>
+  </si>
+  <si>
+    <t>Ex_Mon_Drop_Time</t>
+  </si>
+  <si>
+    <t>Arm_Weapon_Ts_L_Distance</t>
+  </si>
+  <si>
+    <t>Ex_Range_Distance_1</t>
+  </si>
+  <si>
+    <t>Ex_Range_Distance_2</t>
+  </si>
+  <si>
+    <t>Ex_Range_Distance_3</t>
+  </si>
+  <si>
+    <t>Rtec_Timer_End_1</t>
+  </si>
+  <si>
+    <t>Rtec_Timer_End_3</t>
   </si>
 </sst>
 </file>
@@ -1748,7 +1940,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J30"/>
   <sheetViews>
-    <sheetView topLeftCell="A17" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E14" sqref="E14"/>
     </sheetView>
   </sheetViews>
@@ -2845,15 +3037,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B575E61D-8039-463C-8588-67CBC96687A4}">
-  <dimension ref="A1:M288"/>
+  <dimension ref="A1:M318"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <selection activeCell="C257" sqref="C257"/>
+    <sheetView tabSelected="1" topLeftCell="A282" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="A162" sqref="A162:A236"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="31.5703125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="34.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="26.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="19.28515625" bestFit="1" customWidth="1"/>
     <col min="5" max="6" width="19.28515625" customWidth="1"/>
@@ -3277,7 +3469,7 @@
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="3" t="s">
         <v>189</v>
       </c>
       <c r="B21" t="s">
@@ -3577,7 +3769,7 @@
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="A36" s="3" t="s">
         <v>206</v>
       </c>
       <c r="B36" t="s">
@@ -3597,7 +3789,7 @@
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="A37" s="3" t="s">
         <v>207</v>
       </c>
       <c r="B37" t="s">
@@ -3677,7 +3869,7 @@
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+      <c r="A41" s="3" t="s">
         <v>191</v>
       </c>
       <c r="B41" t="s">
@@ -3697,7 +3889,7 @@
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+      <c r="A42" s="3" t="s">
         <v>401</v>
       </c>
       <c r="B42" t="s">
@@ -3880,7 +4072,7 @@
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" t="s">
+      <c r="A51" s="3" t="s">
         <v>229</v>
       </c>
       <c r="B51" t="s">
@@ -3900,7 +4092,7 @@
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+      <c r="A52" s="3" t="s">
         <v>230</v>
       </c>
       <c r="B52" t="s">
@@ -3957,7 +4149,7 @@
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" t="s">
+      <c r="A55" s="3" t="s">
         <v>402</v>
       </c>
       <c r="B55" t="s">
@@ -3977,7 +4169,7 @@
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" t="s">
+      <c r="A56" s="3" t="s">
         <v>407</v>
       </c>
       <c r="B56" t="s">
@@ -3994,7 +4186,7 @@
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" t="s">
+      <c r="A57" s="3" t="s">
         <v>406</v>
       </c>
       <c r="B57" t="s">
@@ -4011,7 +4203,7 @@
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" t="s">
+      <c r="A58" s="3" t="s">
         <v>403</v>
       </c>
       <c r="B58" t="s">
@@ -4031,7 +4223,7 @@
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
+      <c r="A59" s="3" t="s">
         <v>404</v>
       </c>
       <c r="B59" t="s">
@@ -4048,7 +4240,7 @@
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A60" t="s">
+      <c r="A60" s="3" t="s">
         <v>405</v>
       </c>
       <c r="B60" t="s">
@@ -4065,8 +4257,8 @@
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A61" t="s">
-        <v>310</v>
+      <c r="A61" s="3" t="s">
+        <v>455</v>
       </c>
       <c r="B61" t="s">
         <v>5</v>
@@ -4085,8 +4277,8 @@
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A62" t="s">
-        <v>310</v>
+      <c r="A62" s="3" t="s">
+        <v>456</v>
       </c>
       <c r="B62" t="s">
         <v>6</v>
@@ -4102,8 +4294,8 @@
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A63" t="s">
-        <v>310</v>
+      <c r="A63" s="3" t="s">
+        <v>457</v>
       </c>
       <c r="B63" t="s">
         <v>7</v>
@@ -4142,7 +4334,7 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
+      <c r="A65" s="3" t="s">
         <v>233</v>
       </c>
       <c r="B65" t="s">
@@ -4202,7 +4394,7 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A68" t="s">
+      <c r="A68" s="3" t="s">
         <v>236</v>
       </c>
       <c r="B68" t="s">
@@ -4242,7 +4434,7 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A70" t="s">
+      <c r="A70" s="3" t="s">
         <v>238</v>
       </c>
       <c r="B70" t="s">
@@ -4262,7 +4454,7 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A71" t="s">
+      <c r="A71" s="3" t="s">
         <v>239</v>
       </c>
       <c r="B71" t="s">
@@ -4282,7 +4474,7 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A72" t="s">
+      <c r="A72" s="3" t="s">
         <v>240</v>
       </c>
       <c r="B72" t="s">
@@ -4382,7 +4574,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
+      <c r="A77" s="3" t="s">
         <v>254</v>
       </c>
       <c r="B77" t="s">
@@ -4402,7 +4594,7 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A78" t="s">
+      <c r="A78" s="3" t="s">
         <v>255</v>
       </c>
       <c r="B78" t="s">
@@ -4422,7 +4614,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A79" t="s">
+      <c r="A79" s="3" t="s">
         <v>256</v>
       </c>
       <c r="B79" t="s">
@@ -4442,7 +4634,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A80" t="s">
+      <c r="A80" s="3" t="s">
         <v>257</v>
       </c>
       <c r="B80" t="s">
@@ -4462,7 +4654,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A81" t="s">
+      <c r="A81" s="3" t="s">
         <v>241</v>
       </c>
       <c r="B81" t="s">
@@ -4482,7 +4674,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A82" t="s">
+      <c r="A82" s="3" t="s">
         <v>242</v>
       </c>
       <c r="B82" t="s">
@@ -4502,7 +4694,7 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
+      <c r="A83" s="3" t="s">
         <v>243</v>
       </c>
       <c r="B83" t="s">
@@ -4522,7 +4714,7 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
+      <c r="A84" s="3" t="s">
         <v>244</v>
       </c>
       <c r="B84" t="s">
@@ -4542,7 +4734,7 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A85" t="s">
+      <c r="A85" s="3" t="s">
         <v>245</v>
       </c>
       <c r="B85" t="s">
@@ -4562,7 +4754,7 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A86" t="s">
+      <c r="A86" s="3" t="s">
         <v>246</v>
       </c>
       <c r="B86" t="s">
@@ -4582,7 +4774,7 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A87" t="s">
+      <c r="A87" s="3" t="s">
         <v>247</v>
       </c>
       <c r="B87" t="s">
@@ -4602,7 +4794,7 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A88" t="s">
+      <c r="A88" s="3" t="s">
         <v>248</v>
       </c>
       <c r="B88" t="s">
@@ -4642,7 +4834,7 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A90" t="s">
+      <c r="A90" s="3" t="s">
         <v>258</v>
       </c>
       <c r="B90" t="s">
@@ -4662,7 +4854,7 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
+      <c r="A91" s="3" t="s">
         <v>259</v>
       </c>
       <c r="B91" t="s">
@@ -4682,7 +4874,7 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
+      <c r="A92" s="3" t="s">
         <v>260</v>
       </c>
       <c r="B92" t="s">
@@ -4702,7 +4894,7 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A93" t="s">
+      <c r="A93" s="3" t="s">
         <v>261</v>
       </c>
       <c r="B93" t="s">
@@ -4722,7 +4914,7 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A94" t="s">
+      <c r="A94" s="3" t="s">
         <v>262</v>
       </c>
       <c r="B94" t="s">
@@ -4742,7 +4934,7 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A95" t="s">
+      <c r="A95" s="3" t="s">
         <v>263</v>
       </c>
       <c r="B95" t="s">
@@ -4762,7 +4954,7 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A96" t="s">
+      <c r="A96" s="3" t="s">
         <v>264</v>
       </c>
       <c r="B96" t="s">
@@ -4782,7 +4974,7 @@
       </c>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A97" t="s">
+      <c r="A97" s="3" t="s">
         <v>265</v>
       </c>
       <c r="B97" t="s">
@@ -4802,7 +4994,7 @@
       </c>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A98" t="s">
+      <c r="A98" s="3" t="s">
         <v>266</v>
       </c>
       <c r="B98" t="s">
@@ -4822,7 +5014,7 @@
       </c>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A99" t="s">
+      <c r="A99" s="3" t="s">
         <v>267</v>
       </c>
       <c r="B99" t="s">
@@ -4842,7 +5034,7 @@
       </c>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A100" t="s">
+      <c r="A100" s="3" t="s">
         <v>268</v>
       </c>
       <c r="B100" t="s">
@@ -4862,7 +5054,7 @@
       </c>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A101" t="s">
+      <c r="A101" s="3" t="s">
         <v>269</v>
       </c>
       <c r="B101" t="s">
@@ -4882,7 +5074,7 @@
       </c>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A102" t="s">
+      <c r="A102" s="3" t="s">
         <v>270</v>
       </c>
       <c r="B102" t="s">
@@ -4902,7 +5094,7 @@
       </c>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
+      <c r="A103" s="3" t="s">
         <v>271</v>
       </c>
       <c r="B103" t="s">
@@ -4922,7 +5114,7 @@
       </c>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A104" t="s">
+      <c r="A104" s="3" t="s">
         <v>272</v>
       </c>
       <c r="B104" t="s">
@@ -4942,7 +5134,7 @@
       </c>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A105" t="s">
+      <c r="A105" s="3" t="s">
         <v>273</v>
       </c>
       <c r="B105" t="s">
@@ -4962,7 +5154,7 @@
       </c>
     </row>
     <row r="106" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A106" t="s">
+      <c r="A106" s="3" t="s">
         <v>274</v>
       </c>
       <c r="B106" t="s">
@@ -4982,7 +5174,7 @@
       </c>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A107" t="s">
+      <c r="A107" s="3" t="s">
         <v>275</v>
       </c>
       <c r="B107" t="s">
@@ -5002,7 +5194,7 @@
       </c>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A108" t="s">
+      <c r="A108" s="3" t="s">
         <v>276</v>
       </c>
       <c r="B108" t="s">
@@ -5022,7 +5214,7 @@
       </c>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A109" t="s">
+      <c r="A109" s="3" t="s">
         <v>277</v>
       </c>
       <c r="B109" t="s">
@@ -5042,7 +5234,7 @@
       </c>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A110" t="s">
+      <c r="A110" s="3" t="s">
         <v>278</v>
       </c>
       <c r="B110" t="s">
@@ -5062,7 +5254,7 @@
       </c>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A111" t="s">
+      <c r="A111" s="3" t="s">
         <v>279</v>
       </c>
       <c r="B111" t="s">
@@ -5082,7 +5274,7 @@
       </c>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
+      <c r="A112" s="3" t="s">
         <v>280</v>
       </c>
       <c r="B112" t="s">
@@ -5102,7 +5294,7 @@
       </c>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
+      <c r="A113" s="3" t="s">
         <v>281</v>
       </c>
       <c r="B113" t="s">
@@ -5122,7 +5314,7 @@
       </c>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A114" t="s">
+      <c r="A114" s="3" t="s">
         <v>282</v>
       </c>
       <c r="B114" t="s">
@@ -5142,7 +5334,7 @@
       </c>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A115" t="s">
+      <c r="A115" s="3" t="s">
         <v>283</v>
       </c>
       <c r="B115" t="s">
@@ -5162,7 +5354,7 @@
       </c>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A116" t="s">
+      <c r="A116" s="3" t="s">
         <v>284</v>
       </c>
       <c r="B116" t="s">
@@ -5182,7 +5374,7 @@
       </c>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A117" t="s">
+      <c r="A117" s="3" t="s">
         <v>285</v>
       </c>
       <c r="B117" t="s">
@@ -5202,7 +5394,7 @@
       </c>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
+      <c r="A118" s="3" t="s">
         <v>286</v>
       </c>
       <c r="B118" t="s">
@@ -5222,7 +5414,7 @@
       </c>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
+      <c r="A119" s="3" t="s">
         <v>287</v>
       </c>
       <c r="B119" t="s">
@@ -5242,7 +5434,7 @@
       </c>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A120" t="s">
+      <c r="A120" s="3" t="s">
         <v>288</v>
       </c>
       <c r="B120" t="s">
@@ -5262,7 +5454,7 @@
       </c>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A121" t="s">
+      <c r="A121" s="3" t="s">
         <v>289</v>
       </c>
       <c r="B121" t="s">
@@ -5282,7 +5474,7 @@
       </c>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A122" t="s">
+      <c r="A122" s="3" t="s">
         <v>290</v>
       </c>
       <c r="B122" t="s">
@@ -5302,7 +5494,7 @@
       </c>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A123" t="s">
+      <c r="A123" s="3" t="s">
         <v>291</v>
       </c>
       <c r="B123" t="s">
@@ -5322,7 +5514,7 @@
       </c>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A124" t="s">
+      <c r="A124" s="3" t="s">
         <v>292</v>
       </c>
       <c r="B124" t="s">
@@ -5342,7 +5534,7 @@
       </c>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A125" t="s">
+      <c r="A125" s="3" t="s">
         <v>293</v>
       </c>
       <c r="B125" t="s">
@@ -5362,7 +5554,7 @@
       </c>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A126" t="s">
+      <c r="A126" s="3" t="s">
         <v>294</v>
       </c>
       <c r="B126" t="s">
@@ -5382,7 +5574,7 @@
       </c>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A127" t="s">
+      <c r="A127" s="3" t="s">
         <v>295</v>
       </c>
       <c r="B127" t="s">
@@ -5402,7 +5594,7 @@
       </c>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A128" t="s">
+      <c r="A128" s="3" t="s">
         <v>296</v>
       </c>
       <c r="B128" t="s">
@@ -5422,7 +5614,7 @@
       </c>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A129" t="s">
+      <c r="A129" s="3" t="s">
         <v>297</v>
       </c>
       <c r="B129" t="s">
@@ -5442,7 +5634,7 @@
       </c>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A130" t="s">
+      <c r="A130" s="3" t="s">
         <v>298</v>
       </c>
       <c r="B130" t="s">
@@ -5462,7 +5654,7 @@
       </c>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A131" t="s">
+      <c r="A131" s="3" t="s">
         <v>299</v>
       </c>
       <c r="B131" t="s">
@@ -5482,7 +5674,7 @@
       </c>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A132" t="s">
+      <c r="A132" s="3" t="s">
         <v>300</v>
       </c>
       <c r="B132" t="s">
@@ -5502,7 +5694,7 @@
       </c>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A133" t="s">
+      <c r="A133" s="3" t="s">
         <v>301</v>
       </c>
       <c r="B133" t="s">
@@ -5522,7 +5714,7 @@
       </c>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A134" t="s">
+      <c r="A134" s="3" t="s">
         <v>302</v>
       </c>
       <c r="B134" t="s">
@@ -5542,7 +5734,7 @@
       </c>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
+      <c r="A135" s="3" t="s">
         <v>303</v>
       </c>
       <c r="B135" t="s">
@@ -5562,7 +5754,7 @@
       </c>
     </row>
     <row r="136" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A136" t="s">
+      <c r="A136" s="3" t="s">
         <v>304</v>
       </c>
       <c r="B136" t="s">
@@ -5582,7 +5774,7 @@
       </c>
     </row>
     <row r="137" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A137" t="s">
+      <c r="A137" s="3" t="s">
         <v>305</v>
       </c>
       <c r="B137" t="s">
@@ -5602,7 +5794,7 @@
       </c>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A138" t="s">
+      <c r="A138" s="3" t="s">
         <v>306</v>
       </c>
       <c r="B138" t="s">
@@ -5622,7 +5814,7 @@
       </c>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A139" t="s">
+      <c r="A139" s="3" t="s">
         <v>307</v>
       </c>
       <c r="B139" t="s">
@@ -5642,7 +5834,7 @@
       </c>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A140" t="s">
+      <c r="A140" s="3" t="s">
         <v>308</v>
       </c>
       <c r="B140" t="s">
@@ -5662,7 +5854,7 @@
       </c>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
+      <c r="A141" s="3" t="s">
         <v>309</v>
       </c>
       <c r="B141" t="s">
@@ -5741,7 +5933,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="145" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A145" s="3" t="s">
         <v>395</v>
       </c>
@@ -5761,7 +5953,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="146" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A146" s="3" t="s">
         <v>396</v>
       </c>
@@ -5781,7 +5973,7 @@
         <v>313</v>
       </c>
     </row>
-    <row r="147" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A147" s="3" t="s">
         <v>397</v>
       </c>
@@ -5801,9 +5993,9 @@
         <v>313</v>
       </c>
     </row>
-    <row r="148" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A148" t="s">
-        <v>310</v>
+    <row r="148" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A148" s="3" t="s">
+        <v>461</v>
       </c>
       <c r="B148" t="s">
         <v>5</v>
@@ -5815,240 +6007,177 @@
         <v>21</v>
       </c>
     </row>
-    <row r="149" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A149" t="s">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A149" s="3" t="s">
+        <v>462</v>
+      </c>
+      <c r="B149" t="s">
+        <v>5</v>
+      </c>
+      <c r="C149" t="s">
+        <v>48</v>
+      </c>
+      <c r="D149" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="150" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A150" s="3" t="s">
+        <v>463</v>
+      </c>
+      <c r="B150" t="s">
+        <v>5</v>
+      </c>
+      <c r="C150" t="s">
+        <v>48</v>
+      </c>
+      <c r="D150" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="151" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A151" s="3" t="s">
+        <v>464</v>
+      </c>
+      <c r="B151" t="s">
+        <v>5</v>
+      </c>
+      <c r="C151" t="s">
+        <v>48</v>
+      </c>
+      <c r="D151" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="152" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A152" s="3" t="s">
+        <v>465</v>
+      </c>
+      <c r="B152" t="s">
+        <v>5</v>
+      </c>
+      <c r="C152" t="s">
+        <v>48</v>
+      </c>
+      <c r="D152" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="153" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A153" s="3" t="s">
+        <v>466</v>
+      </c>
+      <c r="B153" t="s">
+        <v>5</v>
+      </c>
+      <c r="C153" t="s">
+        <v>48</v>
+      </c>
+      <c r="D153" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="154" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A154" s="3" t="s">
+        <v>467</v>
+      </c>
+      <c r="B154" t="s">
+        <v>5</v>
+      </c>
+      <c r="C154" t="s">
+        <v>48</v>
+      </c>
+      <c r="D154" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="155" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A155" s="3" t="s">
+        <v>468</v>
+      </c>
+      <c r="B155" t="s">
+        <v>5</v>
+      </c>
+      <c r="C155" t="s">
+        <v>48</v>
+      </c>
+      <c r="D155" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="156" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A156" s="3" t="s">
+        <v>469</v>
+      </c>
+      <c r="B156" t="s">
+        <v>5</v>
+      </c>
+      <c r="C156" t="s">
+        <v>48</v>
+      </c>
+      <c r="D156" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="157" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A157" s="3" t="s">
+        <v>470</v>
+      </c>
+      <c r="B157" t="s">
+        <v>5</v>
+      </c>
+      <c r="C157" t="s">
+        <v>48</v>
+      </c>
+      <c r="D157" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="158" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A158" s="3" t="s">
+        <v>471</v>
+      </c>
+      <c r="B158" t="s">
+        <v>5</v>
+      </c>
+      <c r="C158" t="s">
+        <v>48</v>
+      </c>
+      <c r="D158" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="159" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A159" t="s">
         <v>310</v>
       </c>
-      <c r="B149" t="s">
-        <v>6</v>
-      </c>
-      <c r="C149" t="s">
+      <c r="B159" t="s">
+        <v>6</v>
+      </c>
+      <c r="C159" t="s">
         <v>98</v>
       </c>
-      <c r="D149" t="s">
+      <c r="D159" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="150" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A150" t="s">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
         <v>310</v>
       </c>
-      <c r="B150" t="s">
-        <v>7</v>
-      </c>
-      <c r="C150" t="s">
+      <c r="B160" t="s">
+        <v>7</v>
+      </c>
+      <c r="C160" t="s">
         <v>100</v>
       </c>
-      <c r="D150" t="s">
+      <c r="D160" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="151" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A151" t="s">
+    <row r="161" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A161" s="3" t="s">
         <v>190</v>
-      </c>
-      <c r="B151" t="s">
-        <v>5</v>
-      </c>
-      <c r="C151" t="s">
-        <v>49</v>
-      </c>
-      <c r="D151" t="s">
-        <v>22</v>
-      </c>
-      <c r="E151">
-        <v>0</v>
-      </c>
-      <c r="F151" t="s">
-        <v>313</v>
-      </c>
-      <c r="G151" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="152" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A152" s="3" t="s">
-        <v>314</v>
-      </c>
-      <c r="B152" t="s">
-        <v>5</v>
-      </c>
-      <c r="C152" t="s">
-        <v>49</v>
-      </c>
-      <c r="D152" t="s">
-        <v>22</v>
-      </c>
-      <c r="E152">
-        <v>1</v>
-      </c>
-      <c r="G152" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="153" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A153" s="3" t="s">
-        <v>315</v>
-      </c>
-      <c r="B153" t="s">
-        <v>5</v>
-      </c>
-      <c r="C153" t="s">
-        <v>49</v>
-      </c>
-      <c r="D153" t="s">
-        <v>22</v>
-      </c>
-      <c r="E153">
-        <v>2</v>
-      </c>
-      <c r="G153" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="154" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A154" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="B154" t="s">
-        <v>5</v>
-      </c>
-      <c r="C154" t="s">
-        <v>49</v>
-      </c>
-      <c r="D154" t="s">
-        <v>22</v>
-      </c>
-      <c r="E154">
-        <v>3</v>
-      </c>
-      <c r="G154" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="155" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A155" s="3" t="s">
-        <v>317</v>
-      </c>
-      <c r="B155" t="s">
-        <v>5</v>
-      </c>
-      <c r="C155" t="s">
-        <v>49</v>
-      </c>
-      <c r="D155" t="s">
-        <v>22</v>
-      </c>
-      <c r="E155">
-        <v>4</v>
-      </c>
-      <c r="G155" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="156" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A156" s="3" t="s">
-        <v>318</v>
-      </c>
-      <c r="B156" t="s">
-        <v>5</v>
-      </c>
-      <c r="C156" t="s">
-        <v>49</v>
-      </c>
-      <c r="D156" t="s">
-        <v>22</v>
-      </c>
-      <c r="E156">
-        <v>5</v>
-      </c>
-      <c r="G156" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="157" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A157" s="3" t="s">
-        <v>319</v>
-      </c>
-      <c r="B157" t="s">
-        <v>5</v>
-      </c>
-      <c r="C157" t="s">
-        <v>49</v>
-      </c>
-      <c r="D157" t="s">
-        <v>22</v>
-      </c>
-      <c r="E157">
-        <v>6</v>
-      </c>
-      <c r="G157" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="158" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A158" s="3" t="s">
-        <v>320</v>
-      </c>
-      <c r="B158" t="s">
-        <v>5</v>
-      </c>
-      <c r="C158" t="s">
-        <v>49</v>
-      </c>
-      <c r="D158" t="s">
-        <v>22</v>
-      </c>
-      <c r="E158">
-        <v>7</v>
-      </c>
-      <c r="G158" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="159" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A159" s="3" t="s">
-        <v>321</v>
-      </c>
-      <c r="B159" t="s">
-        <v>5</v>
-      </c>
-      <c r="C159" t="s">
-        <v>49</v>
-      </c>
-      <c r="D159" t="s">
-        <v>22</v>
-      </c>
-      <c r="E159">
-        <v>8</v>
-      </c>
-      <c r="G159" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="160" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A160" s="3" t="s">
-        <v>322</v>
-      </c>
-      <c r="B160" t="s">
-        <v>5</v>
-      </c>
-      <c r="C160" t="s">
-        <v>49</v>
-      </c>
-      <c r="D160" t="s">
-        <v>22</v>
-      </c>
-      <c r="E160">
-        <v>9</v>
-      </c>
-      <c r="G160" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="161" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A161" s="3" t="s">
-        <v>329</v>
       </c>
       <c r="B161" t="s">
         <v>5</v>
@@ -6060,12 +6189,18 @@
         <v>22</v>
       </c>
       <c r="E161">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="162" spans="1:5" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="F161" t="s">
+        <v>313</v>
+      </c>
+      <c r="G161" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="3" t="s">
-        <v>330</v>
+        <v>314</v>
       </c>
       <c r="B162" t="s">
         <v>5</v>
@@ -6077,12 +6212,15 @@
         <v>22</v>
       </c>
       <c r="E162">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="163" spans="1:5" x14ac:dyDescent="0.25">
+        <v>1</v>
+      </c>
+      <c r="G162" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="3" t="s">
-        <v>331</v>
+        <v>315</v>
       </c>
       <c r="B163" t="s">
         <v>5</v>
@@ -6094,12 +6232,15 @@
         <v>22</v>
       </c>
       <c r="E163">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="164" spans="1:5" x14ac:dyDescent="0.25">
+        <v>2</v>
+      </c>
+      <c r="G163" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="3" t="s">
-        <v>332</v>
+        <v>316</v>
       </c>
       <c r="B164" t="s">
         <v>5</v>
@@ -6111,12 +6252,15 @@
         <v>22</v>
       </c>
       <c r="E164">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="165" spans="1:5" x14ac:dyDescent="0.25">
+        <v>3</v>
+      </c>
+      <c r="G164" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="3" t="s">
-        <v>333</v>
+        <v>317</v>
       </c>
       <c r="B165" t="s">
         <v>5</v>
@@ -6128,12 +6272,15 @@
         <v>22</v>
       </c>
       <c r="E165">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="166" spans="1:5" x14ac:dyDescent="0.25">
+        <v>4</v>
+      </c>
+      <c r="G165" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="3" t="s">
-        <v>334</v>
+        <v>318</v>
       </c>
       <c r="B166" t="s">
         <v>5</v>
@@ -6145,12 +6292,15 @@
         <v>22</v>
       </c>
       <c r="E166">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="167" spans="1:5" x14ac:dyDescent="0.25">
+        <v>5</v>
+      </c>
+      <c r="G166" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="3" t="s">
-        <v>335</v>
+        <v>319</v>
       </c>
       <c r="B167" t="s">
         <v>5</v>
@@ -6162,12 +6312,15 @@
         <v>22</v>
       </c>
       <c r="E167">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="168" spans="1:5" x14ac:dyDescent="0.25">
+        <v>6</v>
+      </c>
+      <c r="G167" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="3" t="s">
-        <v>336</v>
+        <v>320</v>
       </c>
       <c r="B168" t="s">
         <v>5</v>
@@ -6179,12 +6332,15 @@
         <v>22</v>
       </c>
       <c r="E168">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="169" spans="1:5" x14ac:dyDescent="0.25">
+        <v>7</v>
+      </c>
+      <c r="G168" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="3" t="s">
-        <v>337</v>
+        <v>321</v>
       </c>
       <c r="B169" t="s">
         <v>5</v>
@@ -6196,12 +6352,15 @@
         <v>22</v>
       </c>
       <c r="E169">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="170" spans="1:5" x14ac:dyDescent="0.25">
+        <v>8</v>
+      </c>
+      <c r="G169" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="3" t="s">
-        <v>338</v>
+        <v>322</v>
       </c>
       <c r="B170" t="s">
         <v>5</v>
@@ -6213,12 +6372,15 @@
         <v>22</v>
       </c>
       <c r="E170">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="171" spans="1:5" x14ac:dyDescent="0.25">
+        <v>9</v>
+      </c>
+      <c r="G170" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="3" t="s">
-        <v>339</v>
+        <v>329</v>
       </c>
       <c r="B171" t="s">
         <v>5</v>
@@ -6230,12 +6392,12 @@
         <v>22</v>
       </c>
       <c r="E171">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="172" spans="1:5" x14ac:dyDescent="0.25">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="3" t="s">
-        <v>340</v>
+        <v>330</v>
       </c>
       <c r="B172" t="s">
         <v>5</v>
@@ -6247,12 +6409,12 @@
         <v>22</v>
       </c>
       <c r="E172">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="173" spans="1:5" x14ac:dyDescent="0.25">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="3" t="s">
-        <v>341</v>
+        <v>331</v>
       </c>
       <c r="B173" t="s">
         <v>5</v>
@@ -6264,12 +6426,12 @@
         <v>22</v>
       </c>
       <c r="E173">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="174" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="3" t="s">
-        <v>342</v>
+        <v>332</v>
       </c>
       <c r="B174" t="s">
         <v>5</v>
@@ -6281,12 +6443,12 @@
         <v>22</v>
       </c>
       <c r="E174">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="175" spans="1:5" x14ac:dyDescent="0.25">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="3" t="s">
-        <v>343</v>
+        <v>333</v>
       </c>
       <c r="B175" t="s">
         <v>5</v>
@@ -6298,12 +6460,12 @@
         <v>22</v>
       </c>
       <c r="E175">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="176" spans="1:5" x14ac:dyDescent="0.25">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="3" t="s">
-        <v>344</v>
+        <v>334</v>
       </c>
       <c r="B176" t="s">
         <v>5</v>
@@ -6315,12 +6477,12 @@
         <v>22</v>
       </c>
       <c r="E176">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="177" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A177" s="3" t="s">
-        <v>345</v>
+        <v>335</v>
       </c>
       <c r="B177" t="s">
         <v>5</v>
@@ -6332,12 +6494,12 @@
         <v>22</v>
       </c>
       <c r="E177">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="178" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A178" s="3" t="s">
-        <v>346</v>
+        <v>336</v>
       </c>
       <c r="B178" t="s">
         <v>5</v>
@@ -6349,12 +6511,12 @@
         <v>22</v>
       </c>
       <c r="E178">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="179" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A179" s="3" t="s">
-        <v>347</v>
+        <v>337</v>
       </c>
       <c r="B179" t="s">
         <v>5</v>
@@ -6366,12 +6528,12 @@
         <v>22</v>
       </c>
       <c r="E179">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="180" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A180" s="3" t="s">
-        <v>348</v>
+        <v>338</v>
       </c>
       <c r="B180" t="s">
         <v>5</v>
@@ -6383,12 +6545,12 @@
         <v>22</v>
       </c>
       <c r="E180">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="181" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A181" s="3" t="s">
-        <v>349</v>
+        <v>339</v>
       </c>
       <c r="B181" t="s">
         <v>5</v>
@@ -6400,12 +6562,12 @@
         <v>22</v>
       </c>
       <c r="E181">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="182" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A182" s="3" t="s">
-        <v>350</v>
+        <v>340</v>
       </c>
       <c r="B182" t="s">
         <v>5</v>
@@ -6417,182 +6579,182 @@
         <v>22</v>
       </c>
       <c r="E182">
-        <v>31</v>
+        <v>21</v>
       </c>
     </row>
     <row r="183" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A183" s="3" t="s">
-        <v>351</v>
+        <v>341</v>
       </c>
       <c r="B183" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C183" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D183" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E183">
-        <v>0</v>
+        <v>22</v>
       </c>
     </row>
     <row r="184" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A184" s="3" t="s">
-        <v>352</v>
+        <v>342</v>
       </c>
       <c r="B184" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C184" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D184" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E184">
-        <v>1</v>
+        <v>23</v>
       </c>
     </row>
     <row r="185" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A185" s="3" t="s">
-        <v>353</v>
+        <v>343</v>
       </c>
       <c r="B185" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C185" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D185" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E185">
-        <v>2</v>
+        <v>24</v>
       </c>
     </row>
     <row r="186" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A186" s="3" t="s">
-        <v>354</v>
+        <v>344</v>
       </c>
       <c r="B186" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C186" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D186" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E186">
-        <v>3</v>
+        <v>25</v>
       </c>
     </row>
     <row r="187" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A187" s="3" t="s">
-        <v>355</v>
+        <v>345</v>
       </c>
       <c r="B187" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C187" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D187" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E187">
-        <v>4</v>
+        <v>26</v>
       </c>
     </row>
     <row r="188" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A188" s="3" t="s">
-        <v>380</v>
+        <v>346</v>
       </c>
       <c r="B188" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C188" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D188" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E188">
-        <v>5</v>
+        <v>27</v>
       </c>
     </row>
     <row r="189" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A189" s="3" t="s">
-        <v>381</v>
+        <v>347</v>
       </c>
       <c r="B189" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C189" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D189" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E189">
-        <v>6</v>
+        <v>28</v>
       </c>
     </row>
     <row r="190" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A190" s="3" t="s">
-        <v>382</v>
+        <v>348</v>
       </c>
       <c r="B190" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C190" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D190" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E190">
-        <v>7</v>
+        <v>29</v>
       </c>
     </row>
     <row r="191" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A191" s="3" t="s">
-        <v>383</v>
+        <v>349</v>
       </c>
       <c r="B191" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C191" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D191" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E191">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="192" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A192" s="3" t="s">
-        <v>384</v>
+        <v>350</v>
       </c>
       <c r="B192" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C192" t="s">
-        <v>102</v>
+        <v>49</v>
       </c>
       <c r="D192" t="s">
-        <v>103</v>
+        <v>22</v>
       </c>
       <c r="E192">
-        <v>9</v>
+        <v>31</v>
       </c>
     </row>
     <row r="193" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A193" s="3" t="s">
-        <v>385</v>
+        <v>351</v>
       </c>
       <c r="B193" t="s">
         <v>6</v>
@@ -6604,12 +6766,12 @@
         <v>103</v>
       </c>
       <c r="E193">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="194" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A194" s="3" t="s">
-        <v>386</v>
+        <v>352</v>
       </c>
       <c r="B194" t="s">
         <v>6</v>
@@ -6621,12 +6783,12 @@
         <v>103</v>
       </c>
       <c r="E194">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="195" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A195" s="3" t="s">
-        <v>387</v>
+        <v>353</v>
       </c>
       <c r="B195" t="s">
         <v>6</v>
@@ -6638,12 +6800,12 @@
         <v>103</v>
       </c>
       <c r="E195">
-        <v>12</v>
+        <v>2</v>
       </c>
     </row>
     <row r="196" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A196" s="3" t="s">
-        <v>388</v>
+        <v>354</v>
       </c>
       <c r="B196" t="s">
         <v>6</v>
@@ -6655,12 +6817,12 @@
         <v>103</v>
       </c>
       <c r="E196">
-        <v>13</v>
+        <v>3</v>
       </c>
     </row>
     <row r="197" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A197" t="s">
-        <v>323</v>
+      <c r="A197" s="3" t="s">
+        <v>355</v>
       </c>
       <c r="B197" t="s">
         <v>6</v>
@@ -6672,12 +6834,12 @@
         <v>103</v>
       </c>
       <c r="E197">
-        <v>14</v>
+        <v>4</v>
       </c>
     </row>
     <row r="198" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A198" t="s">
-        <v>324</v>
+      <c r="A198" s="3" t="s">
+        <v>380</v>
       </c>
       <c r="B198" t="s">
         <v>6</v>
@@ -6689,12 +6851,12 @@
         <v>103</v>
       </c>
       <c r="E198">
-        <v>15</v>
+        <v>5</v>
       </c>
     </row>
     <row r="199" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A199" t="s">
-        <v>325</v>
+      <c r="A199" s="3" t="s">
+        <v>381</v>
       </c>
       <c r="B199" t="s">
         <v>6</v>
@@ -6706,12 +6868,12 @@
         <v>103</v>
       </c>
       <c r="E199">
-        <v>16</v>
+        <v>6</v>
       </c>
     </row>
     <row r="200" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A200" t="s">
-        <v>326</v>
+      <c r="A200" s="3" t="s">
+        <v>382</v>
       </c>
       <c r="B200" t="s">
         <v>6</v>
@@ -6723,12 +6885,12 @@
         <v>103</v>
       </c>
       <c r="E200">
-        <v>17</v>
+        <v>7</v>
       </c>
     </row>
     <row r="201" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A201" t="s">
-        <v>327</v>
+      <c r="A201" s="3" t="s">
+        <v>383</v>
       </c>
       <c r="B201" t="s">
         <v>6</v>
@@ -6740,12 +6902,12 @@
         <v>103</v>
       </c>
       <c r="E201">
-        <v>18</v>
+        <v>8</v>
       </c>
     </row>
     <row r="202" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A202" t="s">
-        <v>328</v>
+      <c r="A202" s="3" t="s">
+        <v>384</v>
       </c>
       <c r="B202" t="s">
         <v>6</v>
@@ -6757,12 +6919,12 @@
         <v>103</v>
       </c>
       <c r="E202">
-        <v>19</v>
+        <v>9</v>
       </c>
     </row>
     <row r="203" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A203" t="s">
-        <v>356</v>
+      <c r="A203" s="3" t="s">
+        <v>385</v>
       </c>
       <c r="B203" t="s">
         <v>6</v>
@@ -6774,12 +6936,12 @@
         <v>103</v>
       </c>
       <c r="E203">
-        <v>20</v>
+        <v>10</v>
       </c>
     </row>
     <row r="204" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A204" t="s">
-        <v>357</v>
+      <c r="A204" s="3" t="s">
+        <v>386</v>
       </c>
       <c r="B204" t="s">
         <v>6</v>
@@ -6791,12 +6953,12 @@
         <v>103</v>
       </c>
       <c r="E204">
-        <v>21</v>
+        <v>11</v>
       </c>
     </row>
     <row r="205" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A205" t="s">
-        <v>358</v>
+      <c r="A205" s="3" t="s">
+        <v>387</v>
       </c>
       <c r="B205" t="s">
         <v>6</v>
@@ -6808,12 +6970,12 @@
         <v>103</v>
       </c>
       <c r="E205">
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="206" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A206" t="s">
-        <v>359</v>
+      <c r="A206" s="3" t="s">
+        <v>388</v>
       </c>
       <c r="B206" t="s">
         <v>6</v>
@@ -6825,12 +6987,12 @@
         <v>103</v>
       </c>
       <c r="E206">
-        <v>23</v>
+        <v>13</v>
       </c>
     </row>
     <row r="207" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A207" t="s">
-        <v>360</v>
+      <c r="A207" s="3" t="s">
+        <v>323</v>
       </c>
       <c r="B207" t="s">
         <v>6</v>
@@ -6842,12 +7004,12 @@
         <v>103</v>
       </c>
       <c r="E207">
-        <v>24</v>
+        <v>14</v>
       </c>
     </row>
     <row r="208" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A208" t="s">
-        <v>361</v>
+      <c r="A208" s="3" t="s">
+        <v>324</v>
       </c>
       <c r="B208" t="s">
         <v>6</v>
@@ -6859,12 +7021,12 @@
         <v>103</v>
       </c>
       <c r="E208">
-        <v>25</v>
+        <v>15</v>
       </c>
     </row>
     <row r="209" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A209" t="s">
-        <v>362</v>
+      <c r="A209" s="3" t="s">
+        <v>325</v>
       </c>
       <c r="B209" t="s">
         <v>6</v>
@@ -6876,12 +7038,12 @@
         <v>103</v>
       </c>
       <c r="E209">
-        <v>26</v>
+        <v>16</v>
       </c>
     </row>
     <row r="210" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A210" t="s">
-        <v>363</v>
+      <c r="A210" s="3" t="s">
+        <v>326</v>
       </c>
       <c r="B210" t="s">
         <v>6</v>
@@ -6893,12 +7055,12 @@
         <v>103</v>
       </c>
       <c r="E210">
-        <v>27</v>
+        <v>17</v>
       </c>
     </row>
     <row r="211" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A211" t="s">
-        <v>364</v>
+      <c r="A211" s="3" t="s">
+        <v>327</v>
       </c>
       <c r="B211" t="s">
         <v>6</v>
@@ -6910,12 +7072,12 @@
         <v>103</v>
       </c>
       <c r="E211">
-        <v>28</v>
+        <v>18</v>
       </c>
     </row>
     <row r="212" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A212" t="s">
-        <v>365</v>
+      <c r="A212" s="3" t="s">
+        <v>328</v>
       </c>
       <c r="B212" t="s">
         <v>6</v>
@@ -6927,12 +7089,12 @@
         <v>103</v>
       </c>
       <c r="E212">
-        <v>29</v>
+        <v>19</v>
       </c>
     </row>
     <row r="213" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A213" t="s">
-        <v>366</v>
+      <c r="A213" s="3" t="s">
+        <v>356</v>
       </c>
       <c r="B213" t="s">
         <v>6</v>
@@ -6944,12 +7106,12 @@
         <v>103</v>
       </c>
       <c r="E213">
-        <v>30</v>
+        <v>20</v>
       </c>
     </row>
     <row r="214" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A214" t="s">
-        <v>367</v>
+      <c r="A214" s="3" t="s">
+        <v>357</v>
       </c>
       <c r="B214" t="s">
         <v>6</v>
@@ -6961,182 +7123,182 @@
         <v>103</v>
       </c>
       <c r="E214">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A215" s="3" t="s">
+        <v>358</v>
+      </c>
+      <c r="B215" t="s">
+        <v>6</v>
+      </c>
+      <c r="C215" t="s">
+        <v>102</v>
+      </c>
+      <c r="D215" t="s">
+        <v>103</v>
+      </c>
+      <c r="E215">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A216" s="3" t="s">
+        <v>359</v>
+      </c>
+      <c r="B216" t="s">
+        <v>6</v>
+      </c>
+      <c r="C216" t="s">
+        <v>102</v>
+      </c>
+      <c r="D216" t="s">
+        <v>103</v>
+      </c>
+      <c r="E216">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A217" s="3" t="s">
+        <v>360</v>
+      </c>
+      <c r="B217" t="s">
+        <v>6</v>
+      </c>
+      <c r="C217" t="s">
+        <v>102</v>
+      </c>
+      <c r="D217" t="s">
+        <v>103</v>
+      </c>
+      <c r="E217">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A218" s="3" t="s">
+        <v>361</v>
+      </c>
+      <c r="B218" t="s">
+        <v>6</v>
+      </c>
+      <c r="C218" t="s">
+        <v>102</v>
+      </c>
+      <c r="D218" t="s">
+        <v>103</v>
+      </c>
+      <c r="E218">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A219" s="3" t="s">
+        <v>362</v>
+      </c>
+      <c r="B219" t="s">
+        <v>6</v>
+      </c>
+      <c r="C219" t="s">
+        <v>102</v>
+      </c>
+      <c r="D219" t="s">
+        <v>103</v>
+      </c>
+      <c r="E219">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A220" s="3" t="s">
+        <v>363</v>
+      </c>
+      <c r="B220" t="s">
+        <v>6</v>
+      </c>
+      <c r="C220" t="s">
+        <v>102</v>
+      </c>
+      <c r="D220" t="s">
+        <v>103</v>
+      </c>
+      <c r="E220">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A221" s="3" t="s">
+        <v>364</v>
+      </c>
+      <c r="B221" t="s">
+        <v>6</v>
+      </c>
+      <c r="C221" t="s">
+        <v>102</v>
+      </c>
+      <c r="D221" t="s">
+        <v>103</v>
+      </c>
+      <c r="E221">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A222" s="3" t="s">
+        <v>365</v>
+      </c>
+      <c r="B222" t="s">
+        <v>6</v>
+      </c>
+      <c r="C222" t="s">
+        <v>102</v>
+      </c>
+      <c r="D222" t="s">
+        <v>103</v>
+      </c>
+      <c r="E222">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A223" s="3" t="s">
+        <v>366</v>
+      </c>
+      <c r="B223" t="s">
+        <v>6</v>
+      </c>
+      <c r="C223" t="s">
+        <v>102</v>
+      </c>
+      <c r="D223" t="s">
+        <v>103</v>
+      </c>
+      <c r="E223">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A224" s="3" t="s">
+        <v>367</v>
+      </c>
+      <c r="B224" t="s">
+        <v>6</v>
+      </c>
+      <c r="C224" t="s">
+        <v>102</v>
+      </c>
+      <c r="D224" t="s">
+        <v>103</v>
+      </c>
+      <c r="E224">
         <v>31</v>
       </c>
     </row>
-    <row r="215" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A215" t="s">
+    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A225" s="3" t="s">
         <v>368</v>
-      </c>
-      <c r="B215" t="s">
-        <v>7</v>
-      </c>
-      <c r="C215" t="s">
-        <v>104</v>
-      </c>
-      <c r="D215" t="s">
-        <v>105</v>
-      </c>
-      <c r="E215">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="216" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A216" t="s">
-        <v>369</v>
-      </c>
-      <c r="B216" t="s">
-        <v>7</v>
-      </c>
-      <c r="C216" t="s">
-        <v>104</v>
-      </c>
-      <c r="D216" t="s">
-        <v>105</v>
-      </c>
-      <c r="E216">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="217" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A217" t="s">
-        <v>370</v>
-      </c>
-      <c r="B217" t="s">
-        <v>7</v>
-      </c>
-      <c r="C217" t="s">
-        <v>104</v>
-      </c>
-      <c r="D217" t="s">
-        <v>105</v>
-      </c>
-      <c r="E217">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="218" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A218" t="s">
-        <v>371</v>
-      </c>
-      <c r="B218" t="s">
-        <v>7</v>
-      </c>
-      <c r="C218" t="s">
-        <v>104</v>
-      </c>
-      <c r="D218" t="s">
-        <v>105</v>
-      </c>
-      <c r="E218">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="219" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A219" t="s">
-        <v>372</v>
-      </c>
-      <c r="B219" t="s">
-        <v>7</v>
-      </c>
-      <c r="C219" t="s">
-        <v>104</v>
-      </c>
-      <c r="D219" t="s">
-        <v>105</v>
-      </c>
-      <c r="E219">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="220" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A220" t="s">
-        <v>373</v>
-      </c>
-      <c r="B220" t="s">
-        <v>7</v>
-      </c>
-      <c r="C220" t="s">
-        <v>104</v>
-      </c>
-      <c r="D220" t="s">
-        <v>105</v>
-      </c>
-      <c r="E220">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="221" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A221" t="s">
-        <v>374</v>
-      </c>
-      <c r="B221" t="s">
-        <v>7</v>
-      </c>
-      <c r="C221" t="s">
-        <v>104</v>
-      </c>
-      <c r="D221" t="s">
-        <v>105</v>
-      </c>
-      <c r="E221">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="222" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A222" t="s">
-        <v>375</v>
-      </c>
-      <c r="B222" t="s">
-        <v>7</v>
-      </c>
-      <c r="C222" t="s">
-        <v>104</v>
-      </c>
-      <c r="D222" t="s">
-        <v>105</v>
-      </c>
-      <c r="E222">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="223" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A223" t="s">
-        <v>376</v>
-      </c>
-      <c r="B223" t="s">
-        <v>7</v>
-      </c>
-      <c r="C223" t="s">
-        <v>104</v>
-      </c>
-      <c r="D223" t="s">
-        <v>105</v>
-      </c>
-      <c r="E223">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="224" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A224" t="s">
-        <v>377</v>
-      </c>
-      <c r="B224" t="s">
-        <v>7</v>
-      </c>
-      <c r="C224" t="s">
-        <v>104</v>
-      </c>
-      <c r="D224" t="s">
-        <v>105</v>
-      </c>
-      <c r="E224">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="225" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A225" t="s">
-        <v>378</v>
       </c>
       <c r="B225" t="s">
         <v>7</v>
@@ -7148,12 +7310,12 @@
         <v>105</v>
       </c>
       <c r="E225">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="226" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A226" t="s">
-        <v>379</v>
+      <c r="A226" s="3" t="s">
+        <v>369</v>
       </c>
       <c r="B226" t="s">
         <v>7</v>
@@ -7165,562 +7327,586 @@
         <v>105</v>
       </c>
       <c r="E226">
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="227" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A227" s="3" t="s">
-        <v>416</v>
+        <v>370</v>
       </c>
       <c r="B227" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C227" t="s">
-        <v>50</v>
+        <v>104</v>
       </c>
       <c r="D227" t="s">
-        <v>23</v>
-      </c>
-      <c r="G227" t="s">
-        <v>4</v>
+        <v>105</v>
+      </c>
+      <c r="E227">
+        <v>2</v>
       </c>
     </row>
     <row r="228" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A228" s="3" t="s">
-        <v>417</v>
+        <v>371</v>
       </c>
       <c r="B228" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C228" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D228" t="s">
-        <v>107</v>
+        <v>105</v>
+      </c>
+      <c r="E228">
+        <v>3</v>
       </c>
     </row>
     <row r="229" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A229" s="3" t="s">
-        <v>418</v>
+        <v>372</v>
       </c>
       <c r="B229" t="s">
         <v>7</v>
       </c>
       <c r="C229" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="D229" t="s">
-        <v>109</v>
+        <v>105</v>
+      </c>
+      <c r="E229">
+        <v>4</v>
       </c>
     </row>
     <row r="230" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A230" t="s">
-        <v>310</v>
+      <c r="A230" s="3" t="s">
+        <v>373</v>
       </c>
       <c r="B230" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C230" t="s">
-        <v>51</v>
+        <v>104</v>
       </c>
       <c r="D230" t="s">
-        <v>24</v>
-      </c>
-      <c r="G230" t="s">
-        <v>4</v>
+        <v>105</v>
+      </c>
+      <c r="E230">
+        <v>5</v>
       </c>
     </row>
     <row r="231" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A231" t="s">
-        <v>310</v>
+      <c r="A231" s="3" t="s">
+        <v>374</v>
       </c>
       <c r="B231" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C231" t="s">
-        <v>110</v>
+        <v>104</v>
       </c>
       <c r="D231" t="s">
-        <v>111</v>
+        <v>105</v>
+      </c>
+      <c r="E231">
+        <v>6</v>
       </c>
     </row>
     <row r="232" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A232" t="s">
-        <v>310</v>
+      <c r="A232" s="3" t="s">
+        <v>375</v>
       </c>
       <c r="B232" t="s">
         <v>7</v>
       </c>
       <c r="C232" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D232" t="s">
-        <v>113</v>
+        <v>105</v>
+      </c>
+      <c r="E232">
+        <v>7</v>
       </c>
     </row>
     <row r="233" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A233" t="s">
-        <v>310</v>
+      <c r="A233" s="3" t="s">
+        <v>376</v>
       </c>
       <c r="B233" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C233" t="s">
-        <v>52</v>
+        <v>104</v>
       </c>
       <c r="D233" t="s">
-        <v>25</v>
-      </c>
-      <c r="G233" t="s">
-        <v>4</v>
+        <v>105</v>
+      </c>
+      <c r="E233">
+        <v>8</v>
       </c>
     </row>
     <row r="234" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A234" t="s">
-        <v>310</v>
+      <c r="A234" s="3" t="s">
+        <v>377</v>
       </c>
       <c r="B234" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C234" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
       <c r="D234" t="s">
-        <v>115</v>
+        <v>105</v>
+      </c>
+      <c r="E234">
+        <v>9</v>
       </c>
     </row>
     <row r="235" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A235" t="s">
-        <v>310</v>
+      <c r="A235" s="3" t="s">
+        <v>378</v>
       </c>
       <c r="B235" t="s">
         <v>7</v>
       </c>
       <c r="C235" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
       <c r="D235" t="s">
-        <v>117</v>
+        <v>105</v>
+      </c>
+      <c r="E235">
+        <v>10</v>
       </c>
     </row>
     <row r="236" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A236" s="3" t="s">
-        <v>389</v>
+        <v>379</v>
       </c>
       <c r="B236" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C236" t="s">
-        <v>53</v>
+        <v>104</v>
       </c>
       <c r="D236" t="s">
-        <v>26</v>
-      </c>
-      <c r="G236" t="s">
-        <v>4</v>
+        <v>105</v>
+      </c>
+      <c r="E236">
+        <v>11</v>
       </c>
     </row>
     <row r="237" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A237" s="3" t="s">
-        <v>390</v>
+        <v>416</v>
       </c>
       <c r="B237" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C237" t="s">
-        <v>118</v>
+        <v>50</v>
       </c>
       <c r="D237" t="s">
-        <v>119</v>
+        <v>23</v>
+      </c>
+      <c r="G237" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="238" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A238" s="3" t="s">
-        <v>391</v>
+        <v>417</v>
       </c>
       <c r="B238" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C238" t="s">
-        <v>120</v>
+        <v>106</v>
       </c>
       <c r="D238" t="s">
-        <v>121</v>
+        <v>107</v>
       </c>
     </row>
     <row r="239" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A239" s="3" t="s">
-        <v>413</v>
+        <v>418</v>
       </c>
       <c r="B239" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C239" t="s">
-        <v>54</v>
+        <v>108</v>
       </c>
       <c r="D239" t="s">
-        <v>27</v>
-      </c>
-      <c r="G239" t="s">
-        <v>4</v>
+        <v>109</v>
       </c>
     </row>
     <row r="240" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A240" s="3" t="s">
-        <v>414</v>
+        <v>472</v>
       </c>
       <c r="B240" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C240" t="s">
-        <v>122</v>
+        <v>51</v>
       </c>
       <c r="D240" t="s">
-        <v>123</v>
+        <v>24</v>
+      </c>
+      <c r="F240" t="s">
+        <v>313</v>
+      </c>
+      <c r="G240" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="241" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A241" s="3" t="s">
+        <v>473</v>
+      </c>
+      <c r="B241" t="s">
+        <v>5</v>
+      </c>
+      <c r="C241" t="s">
+        <v>51</v>
+      </c>
+      <c r="D241" t="s">
+        <v>24</v>
+      </c>
+      <c r="F241" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A242" s="3" t="s">
+        <v>474</v>
+      </c>
+      <c r="B242" t="s">
+        <v>6</v>
+      </c>
+      <c r="C242" t="s">
+        <v>110</v>
+      </c>
+      <c r="D242" t="s">
+        <v>111</v>
+      </c>
+      <c r="F242" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A243" s="3" t="s">
+        <v>475</v>
+      </c>
+      <c r="B243" t="s">
+        <v>6</v>
+      </c>
+      <c r="C243" t="s">
+        <v>110</v>
+      </c>
+      <c r="D243" t="s">
+        <v>111</v>
+      </c>
+      <c r="F243" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A244" s="3" t="s">
+        <v>476</v>
+      </c>
+      <c r="B244" t="s">
+        <v>7</v>
+      </c>
+      <c r="C244" t="s">
+        <v>112</v>
+      </c>
+      <c r="D244" t="s">
+        <v>113</v>
+      </c>
+      <c r="F244" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A245" s="3" t="s">
+        <v>477</v>
+      </c>
+      <c r="B245" t="s">
+        <v>7</v>
+      </c>
+      <c r="C245" t="s">
+        <v>112</v>
+      </c>
+      <c r="D245" t="s">
+        <v>113</v>
+      </c>
+      <c r="F245" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A246" s="3" t="s">
+        <v>459</v>
+      </c>
+      <c r="B246" t="s">
+        <v>5</v>
+      </c>
+      <c r="C246" t="s">
+        <v>52</v>
+      </c>
+      <c r="D246" t="s">
+        <v>25</v>
+      </c>
+      <c r="G246" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A247" s="3" t="s">
+        <v>458</v>
+      </c>
+      <c r="B247" t="s">
+        <v>6</v>
+      </c>
+      <c r="C247" t="s">
+        <v>114</v>
+      </c>
+      <c r="D247" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A248" s="3" t="s">
+        <v>460</v>
+      </c>
+      <c r="B248" t="s">
+        <v>7</v>
+      </c>
+      <c r="C248" t="s">
+        <v>116</v>
+      </c>
+      <c r="D248" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A249" s="3" t="s">
+        <v>389</v>
+      </c>
+      <c r="B249" t="s">
+        <v>5</v>
+      </c>
+      <c r="C249" t="s">
+        <v>53</v>
+      </c>
+      <c r="D249" t="s">
+        <v>26</v>
+      </c>
+      <c r="G249" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A250" s="3" t="s">
+        <v>390</v>
+      </c>
+      <c r="B250" t="s">
+        <v>6</v>
+      </c>
+      <c r="C250" t="s">
+        <v>118</v>
+      </c>
+      <c r="D250" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A251" s="3" t="s">
+        <v>391</v>
+      </c>
+      <c r="B251" t="s">
+        <v>7</v>
+      </c>
+      <c r="C251" t="s">
+        <v>120</v>
+      </c>
+      <c r="D251" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A252" s="3" t="s">
+        <v>413</v>
+      </c>
+      <c r="B252" t="s">
+        <v>5</v>
+      </c>
+      <c r="C252" t="s">
+        <v>54</v>
+      </c>
+      <c r="D252" t="s">
+        <v>27</v>
+      </c>
+      <c r="G252" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A253" s="3" t="s">
+        <v>414</v>
+      </c>
+      <c r="B253" t="s">
+        <v>6</v>
+      </c>
+      <c r="C253" t="s">
+        <v>122</v>
+      </c>
+      <c r="D253" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A254" s="3" t="s">
         <v>415</v>
       </c>
-      <c r="B241" t="s">
-        <v>7</v>
-      </c>
-      <c r="C241" t="s">
+      <c r="B254" t="s">
+        <v>7</v>
+      </c>
+      <c r="C254" t="s">
         <v>124</v>
       </c>
-      <c r="D241" t="s">
+      <c r="D254" t="s">
         <v>125</v>
       </c>
     </row>
-    <row r="242" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A242" t="s">
-        <v>310</v>
-      </c>
-      <c r="B242" t="s">
-        <v>5</v>
-      </c>
-      <c r="C242" t="s">
+    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A255" s="3" t="s">
+        <v>447</v>
+      </c>
+      <c r="B255" t="s">
+        <v>5</v>
+      </c>
+      <c r="C255" t="s">
         <v>55</v>
       </c>
-      <c r="D242" t="s">
+      <c r="D255" t="s">
         <v>28</v>
       </c>
-      <c r="G242" t="s">
+      <c r="F255" t="s">
+        <v>422</v>
+      </c>
+      <c r="G255" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="243" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A243" t="s">
-        <v>310</v>
-      </c>
-      <c r="B243" t="s">
-        <v>6</v>
-      </c>
-      <c r="C243" t="s">
-        <v>126</v>
-      </c>
-      <c r="D243" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="244" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A244" t="s">
-        <v>310</v>
-      </c>
-      <c r="B244" t="s">
-        <v>7</v>
-      </c>
-      <c r="C244" t="s">
-        <v>128</v>
-      </c>
-      <c r="D244" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="245" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A245" t="s">
-        <v>310</v>
-      </c>
-      <c r="B245" t="s">
-        <v>5</v>
-      </c>
-      <c r="C245" t="s">
-        <v>56</v>
-      </c>
-      <c r="D245" t="s">
-        <v>29</v>
-      </c>
-      <c r="G245" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="246" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A246" t="s">
-        <v>310</v>
-      </c>
-      <c r="B246" t="s">
-        <v>6</v>
-      </c>
-      <c r="C246" t="s">
-        <v>130</v>
-      </c>
-      <c r="D246" t="s">
-        <v>131</v>
-      </c>
-    </row>
-    <row r="247" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A247" t="s">
-        <v>310</v>
-      </c>
-      <c r="B247" t="s">
-        <v>7</v>
-      </c>
-      <c r="C247" t="s">
-        <v>132</v>
-      </c>
-      <c r="D247" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="248" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A248" t="s">
-        <v>310</v>
-      </c>
-      <c r="B248" t="s">
-        <v>5</v>
-      </c>
-      <c r="C248" t="s">
-        <v>57</v>
-      </c>
-      <c r="D248" t="s">
-        <v>30</v>
-      </c>
-      <c r="G248" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="249" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A249" t="s">
-        <v>310</v>
-      </c>
-      <c r="B249" t="s">
-        <v>6</v>
-      </c>
-      <c r="C249" t="s">
-        <v>134</v>
-      </c>
-      <c r="D249" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="250" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A250" t="s">
-        <v>310</v>
-      </c>
-      <c r="B250" t="s">
-        <v>7</v>
-      </c>
-      <c r="C250" t="s">
-        <v>136</v>
-      </c>
-      <c r="D250" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="251" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A251" t="s">
-        <v>310</v>
-      </c>
-      <c r="B251" t="s">
-        <v>5</v>
-      </c>
-      <c r="C251" t="s">
-        <v>58</v>
-      </c>
-      <c r="D251" t="s">
-        <v>31</v>
-      </c>
-      <c r="G251" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="252" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A252" t="s">
-        <v>310</v>
-      </c>
-      <c r="B252" t="s">
-        <v>6</v>
-      </c>
-      <c r="C252" t="s">
-        <v>138</v>
-      </c>
-      <c r="D252" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="253" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A253" t="s">
-        <v>310</v>
-      </c>
-      <c r="B253" t="s">
-        <v>7</v>
-      </c>
-      <c r="C253" t="s">
-        <v>140</v>
-      </c>
-      <c r="D253" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="254" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A254" t="s">
-        <v>310</v>
-      </c>
-      <c r="B254" t="s">
-        <v>5</v>
-      </c>
-      <c r="C254" t="s">
-        <v>59</v>
-      </c>
-      <c r="D254" t="s">
-        <v>32</v>
-      </c>
-      <c r="G254" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="255" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A255" t="s">
-        <v>310</v>
-      </c>
-      <c r="B255" t="s">
-        <v>6</v>
-      </c>
-      <c r="C255" t="s">
-        <v>142</v>
-      </c>
-      <c r="D255" t="s">
-        <v>143</v>
-      </c>
-    </row>
     <row r="256" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A256" t="s">
-        <v>310</v>
+      <c r="A256" s="3" t="s">
+        <v>448</v>
       </c>
       <c r="B256" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C256" t="s">
-        <v>144</v>
+        <v>55</v>
       </c>
       <c r="D256" t="s">
-        <v>145</v>
+        <v>28</v>
+      </c>
+      <c r="F256" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="257" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A257" s="3" t="s">
-        <v>423</v>
+        <v>494</v>
       </c>
       <c r="B257" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C257" t="s">
-        <v>426</v>
+        <v>126</v>
       </c>
       <c r="D257" t="s">
-        <v>33</v>
-      </c>
-      <c r="F257" t="s">
-        <v>422</v>
-      </c>
-      <c r="G257" t="s">
-        <v>4</v>
+        <v>127</v>
       </c>
     </row>
     <row r="258" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A258" s="3" t="s">
-        <v>429</v>
+        <v>495</v>
       </c>
       <c r="B258" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C258" t="s">
-        <v>426</v>
+        <v>126</v>
       </c>
       <c r="D258" t="s">
-        <v>432</v>
-      </c>
-      <c r="F258" t="s">
-        <v>422</v>
+        <v>127</v>
       </c>
     </row>
     <row r="259" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A259" s="3" t="s">
-        <v>424</v>
+        <v>496</v>
       </c>
       <c r="B259" t="s">
         <v>6</v>
       </c>
       <c r="C259" t="s">
-        <v>427</v>
+        <v>126</v>
       </c>
       <c r="D259" t="s">
-        <v>146</v>
-      </c>
-      <c r="F259" t="s">
-        <v>422</v>
+        <v>127</v>
       </c>
     </row>
     <row r="260" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A260" s="3" t="s">
-        <v>431</v>
+      <c r="A260" t="s">
+        <v>310</v>
       </c>
       <c r="B260" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C260" t="s">
-        <v>427</v>
+        <v>128</v>
       </c>
       <c r="D260" t="s">
-        <v>433</v>
-      </c>
-      <c r="F260" t="s">
-        <v>422</v>
+        <v>129</v>
       </c>
     </row>
     <row r="261" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A261" s="3" t="s">
-        <v>425</v>
+        <v>449</v>
       </c>
       <c r="B261" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C261" t="s">
-        <v>428</v>
+        <v>56</v>
       </c>
       <c r="D261" t="s">
-        <v>147</v>
-      </c>
-      <c r="F261" t="s">
-        <v>422</v>
+        <v>29</v>
+      </c>
+      <c r="G261" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="262" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A262" s="3" t="s">
-        <v>430</v>
+        <v>450</v>
       </c>
       <c r="B262" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C262" t="s">
-        <v>428</v>
+        <v>56</v>
       </c>
       <c r="D262" t="s">
-        <v>434</v>
-      </c>
-      <c r="F262" t="s">
-        <v>422</v>
+        <v>29</v>
       </c>
     </row>
     <row r="263" spans="1:7" x14ac:dyDescent="0.25">
@@ -7728,16 +7914,13 @@
         <v>310</v>
       </c>
       <c r="B263" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C263" t="s">
-        <v>60</v>
+        <v>130</v>
       </c>
       <c r="D263" t="s">
-        <v>34</v>
-      </c>
-      <c r="G263" t="s">
-        <v>4</v>
+        <v>131</v>
       </c>
     </row>
     <row r="264" spans="1:7" x14ac:dyDescent="0.25">
@@ -7745,131 +7928,137 @@
         <v>310</v>
       </c>
       <c r="B264" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C264" t="s">
-        <v>148</v>
+        <v>132</v>
       </c>
       <c r="D264" t="s">
-        <v>149</v>
+        <v>133</v>
       </c>
     </row>
     <row r="265" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A265" t="s">
-        <v>310</v>
+      <c r="A265" s="3" t="s">
+        <v>451</v>
       </c>
       <c r="B265" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C265" t="s">
-        <v>150</v>
+        <v>57</v>
       </c>
       <c r="D265" t="s">
-        <v>151</v>
+        <v>30</v>
+      </c>
+      <c r="G265" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="266" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A266" t="s">
-        <v>310</v>
+      <c r="A266" s="3" t="s">
+        <v>452</v>
       </c>
       <c r="B266" t="s">
         <v>5</v>
       </c>
       <c r="C266" t="s">
-        <v>61</v>
+        <v>57</v>
       </c>
       <c r="D266" t="s">
-        <v>35</v>
-      </c>
-      <c r="G266" t="s">
-        <v>4</v>
+        <v>30</v>
       </c>
     </row>
     <row r="267" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A267" t="s">
-        <v>310</v>
+      <c r="A267" s="3" t="s">
+        <v>454</v>
       </c>
       <c r="B267" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C267" t="s">
-        <v>152</v>
+        <v>57</v>
       </c>
       <c r="D267" t="s">
-        <v>153</v>
+        <v>30</v>
       </c>
     </row>
     <row r="268" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A268" t="s">
-        <v>310</v>
+      <c r="A268" s="3" t="s">
+        <v>487</v>
       </c>
       <c r="B268" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C268" t="s">
-        <v>154</v>
+        <v>134</v>
       </c>
       <c r="D268" t="s">
-        <v>155</v>
+        <v>135</v>
+      </c>
+      <c r="F268" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="269" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A269" t="s">
-        <v>310</v>
+      <c r="A269" s="3" t="s">
+        <v>488</v>
       </c>
       <c r="B269" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C269" t="s">
-        <v>62</v>
+        <v>134</v>
       </c>
       <c r="D269" t="s">
-        <v>36</v>
-      </c>
-      <c r="G269" t="s">
-        <v>4</v>
+        <v>135</v>
+      </c>
+      <c r="F269" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="270" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A270" t="s">
-        <v>310</v>
+      <c r="A270" s="3" t="s">
+        <v>489</v>
       </c>
       <c r="B270" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="C270" t="s">
-        <v>156</v>
+        <v>136</v>
       </c>
       <c r="D270" t="s">
-        <v>157</v>
+        <v>137</v>
       </c>
     </row>
     <row r="271" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A271" t="s">
-        <v>310</v>
+      <c r="A271" s="3" t="s">
+        <v>490</v>
       </c>
       <c r="B271" t="s">
         <v>7</v>
       </c>
       <c r="C271" t="s">
-        <v>158</v>
+        <v>136</v>
       </c>
       <c r="D271" t="s">
-        <v>159</v>
+        <v>137</v>
       </c>
     </row>
     <row r="272" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A272" s="3" t="s">
-        <v>408</v>
+        <v>478</v>
       </c>
       <c r="B272" t="s">
         <v>5</v>
       </c>
       <c r="C272" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D272" t="s">
-        <v>37</v>
+        <v>31</v>
+      </c>
+      <c r="F272" t="s">
+        <v>422</v>
       </c>
       <c r="G272" t="s">
         <v>4</v>
@@ -7877,120 +8066,138 @@
     </row>
     <row r="273" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A273" s="3" t="s">
-        <v>409</v>
+        <v>479</v>
       </c>
       <c r="B273" t="s">
         <v>5</v>
       </c>
       <c r="C273" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D273" t="s">
-        <v>411</v>
+        <v>31</v>
+      </c>
+      <c r="F273" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="274" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A274" s="3" t="s">
-        <v>410</v>
+        <v>480</v>
       </c>
       <c r="B274" t="s">
         <v>5</v>
       </c>
       <c r="C274" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="D274" t="s">
-        <v>412</v>
+        <v>31</v>
+      </c>
+      <c r="F274" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="275" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A275" t="s">
-        <v>310</v>
+      <c r="A275" s="3" t="s">
+        <v>481</v>
       </c>
       <c r="B275" t="s">
         <v>6</v>
       </c>
       <c r="C275" t="s">
-        <v>160</v>
+        <v>138</v>
       </c>
       <c r="D275" t="s">
-        <v>161</v>
+        <v>139</v>
+      </c>
+      <c r="F275" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="276" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A276" t="s">
-        <v>310</v>
+      <c r="A276" s="3" t="s">
+        <v>482</v>
       </c>
       <c r="B276" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C276" t="s">
-        <v>162</v>
+        <v>138</v>
       </c>
       <c r="D276" t="s">
-        <v>163</v>
+        <v>139</v>
+      </c>
+      <c r="F276" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="277" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A277" t="s">
-        <v>310</v>
+      <c r="A277" s="3" t="s">
+        <v>483</v>
       </c>
       <c r="B277" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C277" t="s">
-        <v>64</v>
+        <v>138</v>
       </c>
       <c r="D277" t="s">
-        <v>38</v>
-      </c>
-      <c r="G277" t="s">
-        <v>4</v>
+        <v>139</v>
+      </c>
+      <c r="F277" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="278" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A278" t="s">
-        <v>310</v>
+      <c r="A278" s="3" t="s">
+        <v>484</v>
       </c>
       <c r="B278" t="s">
         <v>6</v>
       </c>
       <c r="C278" t="s">
-        <v>164</v>
+        <v>138</v>
       </c>
       <c r="D278" t="s">
-        <v>165</v>
+        <v>139</v>
+      </c>
+      <c r="F278" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="279" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A279" t="s">
-        <v>310</v>
+      <c r="A279" s="3" t="s">
+        <v>485</v>
       </c>
       <c r="B279" t="s">
         <v>7</v>
       </c>
       <c r="C279" t="s">
-        <v>166</v>
+        <v>140</v>
       </c>
       <c r="D279" t="s">
-        <v>167</v>
+        <v>141</v>
+      </c>
+      <c r="F279" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="280" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A280" t="s">
-        <v>310</v>
+      <c r="A280" s="3" t="s">
+        <v>486</v>
       </c>
       <c r="B280" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C280" t="s">
-        <v>65</v>
+        <v>140</v>
       </c>
       <c r="D280" t="s">
-        <v>39</v>
-      </c>
-      <c r="G280" t="s">
-        <v>4</v>
+        <v>141</v>
+      </c>
+      <c r="F280" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="281" spans="1:7" x14ac:dyDescent="0.25">
@@ -7998,13 +8205,16 @@
         <v>310</v>
       </c>
       <c r="B281" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="C281" t="s">
-        <v>168</v>
+        <v>59</v>
       </c>
       <c r="D281" t="s">
-        <v>169</v>
+        <v>32</v>
+      </c>
+      <c r="G281" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="282" spans="1:7" x14ac:dyDescent="0.25">
@@ -8012,13 +8222,13 @@
         <v>310</v>
       </c>
       <c r="B282" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C282" t="s">
-        <v>170</v>
+        <v>142</v>
       </c>
       <c r="D282" t="s">
-        <v>171</v>
+        <v>143</v>
       </c>
     </row>
     <row r="283" spans="1:7" x14ac:dyDescent="0.25">
@@ -8026,97 +8236,571 @@
         <v>310</v>
       </c>
       <c r="B283" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="C283" t="s">
-        <v>66</v>
+        <v>144</v>
       </c>
       <c r="D283" t="s">
-        <v>40</v>
-      </c>
-      <c r="G283" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A284" s="3" t="s">
+        <v>423</v>
+      </c>
+      <c r="B284" t="s">
+        <v>5</v>
+      </c>
+      <c r="C284" t="s">
+        <v>426</v>
+      </c>
+      <c r="D284" t="s">
+        <v>33</v>
+      </c>
+      <c r="F284" t="s">
+        <v>422</v>
+      </c>
+      <c r="G284" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="284" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A284" t="s">
-        <v>310</v>
-      </c>
-      <c r="B284" t="s">
-        <v>6</v>
-      </c>
-      <c r="C284" t="s">
-        <v>172</v>
-      </c>
-      <c r="D284" t="s">
-        <v>173</v>
-      </c>
-    </row>
     <row r="285" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A285" t="s">
-        <v>310</v>
+      <c r="A285" s="3" t="s">
+        <v>429</v>
       </c>
       <c r="B285" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C285" t="s">
-        <v>174</v>
+        <v>426</v>
       </c>
       <c r="D285" t="s">
-        <v>175</v>
+        <v>432</v>
+      </c>
+      <c r="F285" t="s">
+        <v>422</v>
       </c>
     </row>
     <row r="286" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A286" t="s">
-        <v>419</v>
+      <c r="A286" s="3" t="s">
+        <v>424</v>
       </c>
       <c r="B286" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="C286" t="s">
-        <v>67</v>
+        <v>427</v>
       </c>
       <c r="D286" t="s">
-        <v>41</v>
+        <v>146</v>
       </c>
       <c r="F286" t="s">
         <v>422</v>
       </c>
-      <c r="G286" t="s">
-        <v>4</v>
-      </c>
     </row>
     <row r="287" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A287" t="s">
-        <v>420</v>
+      <c r="A287" s="3" t="s">
+        <v>431</v>
       </c>
       <c r="B287" t="s">
         <v>6</v>
       </c>
       <c r="C287" t="s">
-        <v>176</v>
+        <v>427</v>
       </c>
       <c r="D287" t="s">
-        <v>177</v>
+        <v>433</v>
       </c>
       <c r="F287" t="s">
         <v>422</v>
       </c>
     </row>
     <row r="288" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A288" t="s">
+      <c r="A288" s="3" t="s">
+        <v>425</v>
+      </c>
+      <c r="B288" t="s">
+        <v>7</v>
+      </c>
+      <c r="C288" t="s">
+        <v>428</v>
+      </c>
+      <c r="D288" t="s">
+        <v>147</v>
+      </c>
+      <c r="F288" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="289" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A289" s="3" t="s">
+        <v>430</v>
+      </c>
+      <c r="B289" t="s">
+        <v>7</v>
+      </c>
+      <c r="C289" t="s">
+        <v>428</v>
+      </c>
+      <c r="D289" t="s">
+        <v>434</v>
+      </c>
+      <c r="F289" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="290" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A290" s="3" t="s">
+        <v>453</v>
+      </c>
+      <c r="B290" t="s">
+        <v>5</v>
+      </c>
+      <c r="C290" t="s">
+        <v>60</v>
+      </c>
+      <c r="D290" t="s">
+        <v>34</v>
+      </c>
+      <c r="G290" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="291" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A291" t="s">
+        <v>497</v>
+      </c>
+      <c r="B291" t="s">
+        <v>6</v>
+      </c>
+      <c r="C291" t="s">
+        <v>148</v>
+      </c>
+      <c r="D291" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="292" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A292" t="s">
+        <v>498</v>
+      </c>
+      <c r="B292" t="s">
+        <v>7</v>
+      </c>
+      <c r="C292" t="s">
+        <v>150</v>
+      </c>
+      <c r="D292" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="293" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A293" s="3" t="s">
+        <v>491</v>
+      </c>
+      <c r="B293" t="s">
+        <v>5</v>
+      </c>
+      <c r="C293" t="s">
+        <v>61</v>
+      </c>
+      <c r="D293" t="s">
+        <v>35</v>
+      </c>
+      <c r="G293" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="294" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A294" s="3" t="s">
+        <v>492</v>
+      </c>
+      <c r="B294" t="s">
+        <v>6</v>
+      </c>
+      <c r="C294" t="s">
+        <v>152</v>
+      </c>
+      <c r="D294" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="295" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A295" t="s">
+        <v>310</v>
+      </c>
+      <c r="B295" t="s">
+        <v>7</v>
+      </c>
+      <c r="C295" t="s">
+        <v>154</v>
+      </c>
+      <c r="D295" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="296" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A296" t="s">
+        <v>310</v>
+      </c>
+      <c r="B296" t="s">
+        <v>5</v>
+      </c>
+      <c r="C296" t="s">
+        <v>62</v>
+      </c>
+      <c r="D296" t="s">
+        <v>36</v>
+      </c>
+      <c r="G296" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="297" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A297" t="s">
+        <v>310</v>
+      </c>
+      <c r="B297" t="s">
+        <v>6</v>
+      </c>
+      <c r="C297" t="s">
+        <v>156</v>
+      </c>
+      <c r="D297" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="298" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A298" t="s">
+        <v>310</v>
+      </c>
+      <c r="B298" t="s">
+        <v>7</v>
+      </c>
+      <c r="C298" t="s">
+        <v>158</v>
+      </c>
+      <c r="D298" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="299" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A299" s="3" t="s">
+        <v>408</v>
+      </c>
+      <c r="B299" t="s">
+        <v>5</v>
+      </c>
+      <c r="C299" t="s">
+        <v>63</v>
+      </c>
+      <c r="D299" t="s">
+        <v>37</v>
+      </c>
+      <c r="G299" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="300" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A300" s="3" t="s">
+        <v>409</v>
+      </c>
+      <c r="B300" t="s">
+        <v>5</v>
+      </c>
+      <c r="C300" t="s">
+        <v>63</v>
+      </c>
+      <c r="D300" t="s">
+        <v>411</v>
+      </c>
+    </row>
+    <row r="301" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A301" s="3" t="s">
+        <v>410</v>
+      </c>
+      <c r="B301" t="s">
+        <v>5</v>
+      </c>
+      <c r="C301" t="s">
+        <v>63</v>
+      </c>
+      <c r="D301" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="302" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A302" s="3" t="s">
+        <v>493</v>
+      </c>
+      <c r="B302" t="s">
+        <v>6</v>
+      </c>
+      <c r="C302" t="s">
+        <v>160</v>
+      </c>
+      <c r="D302" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="303" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A303" t="s">
+        <v>310</v>
+      </c>
+      <c r="B303" t="s">
+        <v>7</v>
+      </c>
+      <c r="C303" t="s">
+        <v>162</v>
+      </c>
+      <c r="D303" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="304" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A304" s="3" t="s">
+        <v>441</v>
+      </c>
+      <c r="B304" t="s">
+        <v>5</v>
+      </c>
+      <c r="C304" t="s">
+        <v>64</v>
+      </c>
+      <c r="D304" t="s">
+        <v>38</v>
+      </c>
+      <c r="F304" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="305" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A305" s="3" t="s">
+        <v>442</v>
+      </c>
+      <c r="B305" t="s">
+        <v>5</v>
+      </c>
+      <c r="C305" t="s">
+        <v>64</v>
+      </c>
+      <c r="D305" t="s">
+        <v>38</v>
+      </c>
+      <c r="F305" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="306" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A306" s="3" t="s">
+        <v>443</v>
+      </c>
+      <c r="B306" t="s">
+        <v>6</v>
+      </c>
+      <c r="C306" t="s">
+        <v>164</v>
+      </c>
+      <c r="D306" t="s">
+        <v>165</v>
+      </c>
+      <c r="F306" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="307" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A307" s="3" t="s">
+        <v>444</v>
+      </c>
+      <c r="B307" t="s">
+        <v>6</v>
+      </c>
+      <c r="C307" t="s">
+        <v>164</v>
+      </c>
+      <c r="D307" t="s">
+        <v>165</v>
+      </c>
+      <c r="F307" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="308" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A308" s="3" t="s">
+        <v>445</v>
+      </c>
+      <c r="B308" t="s">
+        <v>7</v>
+      </c>
+      <c r="C308" t="s">
+        <v>166</v>
+      </c>
+      <c r="D308" t="s">
+        <v>167</v>
+      </c>
+      <c r="F308" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="309" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A309" s="3" t="s">
+        <v>446</v>
+      </c>
+      <c r="B309" t="s">
+        <v>7</v>
+      </c>
+      <c r="C309" t="s">
+        <v>166</v>
+      </c>
+      <c r="D309" t="s">
+        <v>167</v>
+      </c>
+      <c r="F309" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="310" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A310" s="3" t="s">
+        <v>435</v>
+      </c>
+      <c r="B310" t="s">
+        <v>5</v>
+      </c>
+      <c r="C310" t="s">
+        <v>65</v>
+      </c>
+      <c r="D310" t="s">
+        <v>39</v>
+      </c>
+      <c r="G310" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="311" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A311" s="3" t="s">
+        <v>437</v>
+      </c>
+      <c r="B311" t="s">
+        <v>6</v>
+      </c>
+      <c r="C311" t="s">
+        <v>168</v>
+      </c>
+      <c r="D311" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="312" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A312" s="3" t="s">
+        <v>436</v>
+      </c>
+      <c r="B312" t="s">
+        <v>7</v>
+      </c>
+      <c r="C312" t="s">
+        <v>170</v>
+      </c>
+      <c r="D312" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="313" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A313" s="3" t="s">
+        <v>438</v>
+      </c>
+      <c r="B313" t="s">
+        <v>5</v>
+      </c>
+      <c r="C313" t="s">
+        <v>66</v>
+      </c>
+      <c r="D313" t="s">
+        <v>40</v>
+      </c>
+      <c r="G313" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="314" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A314" s="3" t="s">
+        <v>439</v>
+      </c>
+      <c r="B314" t="s">
+        <v>6</v>
+      </c>
+      <c r="C314" t="s">
+        <v>172</v>
+      </c>
+      <c r="D314" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="315" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A315" s="3" t="s">
+        <v>440</v>
+      </c>
+      <c r="B315" t="s">
+        <v>7</v>
+      </c>
+      <c r="C315" t="s">
+        <v>174</v>
+      </c>
+      <c r="D315" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="316" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A316" s="3" t="s">
+        <v>419</v>
+      </c>
+      <c r="B316" t="s">
+        <v>5</v>
+      </c>
+      <c r="C316" t="s">
+        <v>67</v>
+      </c>
+      <c r="D316" t="s">
+        <v>41</v>
+      </c>
+      <c r="F316" t="s">
+        <v>422</v>
+      </c>
+      <c r="G316" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="317" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A317" s="3" t="s">
+        <v>420</v>
+      </c>
+      <c r="B317" t="s">
+        <v>6</v>
+      </c>
+      <c r="C317" t="s">
+        <v>176</v>
+      </c>
+      <c r="D317" t="s">
+        <v>177</v>
+      </c>
+      <c r="F317" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="318" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A318" s="3" t="s">
         <v>421</v>
       </c>
-      <c r="B288" t="s">
-        <v>7</v>
-      </c>
-      <c r="C288" t="s">
+      <c r="B318" t="s">
+        <v>7</v>
+      </c>
+      <c r="C318" t="s">
         <v>178</v>
       </c>
-      <c r="D288" t="s">
+      <c r="D318" t="s">
         <v>179</v>
       </c>
-      <c r="F288" t="s">
+      <c r="F318" t="s">
         <v>422</v>
       </c>
     </row>

</xml_diff>